<commit_message>
add info of length of chain
</commit_message>
<xml_diff>
--- a/result_q1.xlsx
+++ b/result_q1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-linjiang\Documents\MATLAB\系泊系统设计\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-linjiang\Documents\MATLAB\mooring-system-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FED284E5-1DAD-4286-9040-086A356FC5C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C865F259-DCA2-477C-878E-265267A68462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{9A052B15-2FF8-4417-AE4B-5A829C725600}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>曲线参数a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,6 +149,10 @@
   </si>
   <si>
     <t>18.5011°</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锚链长度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EA553C-56B9-4C4C-91C3-DC53B9D81698}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -665,6 +669,20 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>15.236700000000001</v>
+      </c>
+      <c r="C11">
+        <v>21.722899999999999</v>
+      </c>
+      <c r="D11">
+        <v>22.05</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>